<commit_message>
cambios de reportes y validaciones
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaCnpc.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaCnpc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181CA217-EC9E-4DD7-A0AE-668A065C5239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47331E14-E704-4713-B4D1-5600413FF919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8A21D80-6B9E-470C-B871-94B7E315DE21}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <definedName name="_TTA1">#REF!</definedName>
     <definedName name="_TTD2">#REF!</definedName>
     <definedName name="AAA">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Boleta_CNPC!$B$1:$J$59</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Boleta_CNPC!$B$1:$J$74</definedName>
     <definedName name="_xlnm.Database">'[4]TABLA TRINITY'!#REF!</definedName>
     <definedName name="BBB">#REF!</definedName>
     <definedName name="CCC">#REF!</definedName>
@@ -782,11 +782,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -853,9 +850,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -880,9 +874,6 @@
     </xf>
     <xf numFmtId="4" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -911,9 +902,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -964,8 +952,45 @@
     <xf numFmtId="166" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -973,10 +998,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -986,15 +1011,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1041,6 +1057,30 @@
     </xf>
     <xf numFmtId="4" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -30042,783 +30082,993 @@
   <sheetPr codeName="Hoja40">
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="10"/>
-    <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="34" style="9" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="4" style="4"/>
-    <col min="12" max="12" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="4" style="4"/>
-    <col min="20" max="20" width="31.5703125" style="4" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" style="4" customWidth="1"/>
-    <col min="22" max="16384" width="4" style="4"/>
+    <col min="1" max="1" width="4" style="9"/>
+    <col min="2" max="2" width="7.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="34" style="8" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="4" style="3"/>
+    <col min="12" max="12" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="4" style="3"/>
+    <col min="20" max="20" width="31.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="4" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="78"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="84" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="3" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="3"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="80"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="74" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="75"/>
-      <c r="K2" s="6"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="82"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="8" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
+      <c r="B4" s="61"/>
+      <c r="J4" s="64"/>
     </row>
     <row r="5" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="4" t="s">
+      <c r="B5" s="62"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="J5" s="65"/>
     </row>
     <row r="6" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="13"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="65"/>
     </row>
     <row r="7" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="62"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>6</v>
       </c>
+      <c r="J7" s="65"/>
     </row>
     <row r="8" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="15" t="str">
+      <c r="B8" s="62"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="14" t="str">
         <f>+I5</f>
         <v>{{DiaOperativo}}</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>60</v>
       </c>
+      <c r="J8" s="65"/>
     </row>
     <row r="9" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="13"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="65"/>
     </row>
     <row r="10" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="62"/>
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="65"/>
     </row>
     <row r="11" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="21"/>
+      <c r="B11" s="62"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="65"/>
     </row>
     <row r="12" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="22" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="J12" s="65"/>
     </row>
     <row r="13" spans="2:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="4"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="65"/>
     </row>
     <row r="14" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="22" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="65"/>
     </row>
     <row r="15" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="25"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="24"/>
+      <c r="J15" s="65"/>
     </row>
     <row r="16" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="66" t="s">
+      <c r="B16" s="63"/>
+      <c r="C16" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="65"/>
     </row>
     <row r="17" spans="1:21" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="29" t="s">
+      <c r="B17" s="62"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="30" t="s">
+      <c r="H17" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="28" t="s">
         <v>18</v>
       </c>
+      <c r="J17" s="65"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="29" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
+      <c r="J18" s="65"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
     </row>
     <row r="19" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-      <c r="C19" s="37" t="s">
+      <c r="B19" s="62"/>
+      <c r="C19" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="35" t="s">
+      <c r="I19" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="J19" s="36"/>
+      <c r="J19" s="66"/>
     </row>
     <row r="20" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="66"/>
     </row>
     <row r="21" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="40"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="36"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="37"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="66"/>
     </row>
-    <row r="22" spans="1:21" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="39" t="s">
+    <row r="22" spans="1:21" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="11"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="67"/>
     </row>
-    <row r="23" spans="1:21" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="11"/>
+    <row r="23" spans="1:21" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="67"/>
     </row>
-    <row r="24" spans="1:21" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="73" t="s">
+    <row r="24" spans="1:21" s="36" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="73"/>
-      <c r="E24" s="90" t="s">
+      <c r="D24" s="78"/>
+      <c r="E24" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="11"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="67"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="39" t="s">
+      <c r="B25" s="63"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="65"/>
     </row>
-    <row r="26" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="63"/>
+      <c r="J26" s="65"/>
+    </row>
     <row r="27" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="66" t="s">
+      <c r="B27" s="63"/>
+      <c r="C27" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="70" t="s">
+      <c r="E27" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="28"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="65"/>
     </row>
     <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="70" t="s">
+      <c r="B28" s="63"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="70" t="s">
+      <c r="G28" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="70" t="s">
+      <c r="H28" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="70" t="s">
+      <c r="I28" s="79" t="s">
         <v>27</v>
       </c>
+      <c r="J28" s="65"/>
     </row>
     <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="80"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="65"/>
     </row>
     <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="65"/>
     </row>
     <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="71"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="65"/>
     </row>
     <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="65"/>
     </row>
-    <row r="33" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
+    <row r="33" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B33" s="63"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="81"/>
+      <c r="J33" s="65"/>
     </row>
-    <row r="34" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="59" t="s">
+    <row r="34" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B34" s="63"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="59" t="s">
+      <c r="F34" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="59" t="s">
+      <c r="G34" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="59" t="s">
+      <c r="H34" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="59" t="s">
+      <c r="I34" s="55" t="s">
         <v>32</v>
       </c>
+      <c r="J34" s="65"/>
     </row>
-    <row r="35" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C35" s="37" t="s">
+    <row r="35" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B35" s="63"/>
+      <c r="C35" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="33" t="s">
+      <c r="F35" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="34" t="s">
+      <c r="G35" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="H35" s="33" t="s">
+      <c r="H35" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="35" t="s">
+      <c r="I35" s="33" t="s">
         <v>69</v>
       </c>
+      <c r="J35" s="65"/>
     </row>
-    <row r="36" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="38"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="44"/>
+    <row r="36" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="63"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="65"/>
     </row>
-    <row r="37" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D37" s="39"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="24"/>
+    <row r="37" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="63"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="65"/>
     </row>
-    <row r="38" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="11" t="s">
+    <row r="38" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="63"/>
+      <c r="C38" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="65"/>
     </row>
-    <row r="39" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
+    <row r="39" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="63"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="65"/>
     </row>
-    <row r="40" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="4"/>
-      <c r="D40" s="22" t="s">
+    <row r="40" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="63"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G40" s="45"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="65"/>
     </row>
-    <row r="41" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="4"/>
-      <c r="D41" s="22" t="s">
+    <row r="41" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="63"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G41" s="45"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="65"/>
     </row>
-    <row r="42" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="4"/>
-      <c r="D42" s="70" t="s">
+    <row r="42" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="63"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="76" t="s">
+      <c r="E42" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="65"/>
     </row>
-    <row r="43" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C43" s="4"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="4" t="s">
+    <row r="43" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B43" s="63"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="83"/>
+      <c r="F43" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="65"/>
     </row>
-    <row r="45" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="66" t="s">
+    <row r="44" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="63"/>
+      <c r="J44" s="65"/>
+    </row>
+    <row r="45" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="63"/>
+      <c r="C45" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="66" t="s">
+      <c r="D45" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="E45" s="67" t="s">
+      <c r="E45" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="27" t="s">
+      <c r="F45" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="28"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="65"/>
     </row>
-    <row r="46" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="66"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="73" t="s">
+    <row r="46" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="63"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="G46" s="73" t="s">
+      <c r="G46" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="H46" s="73" t="s">
+      <c r="H46" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="I46" s="73" t="s">
+      <c r="I46" s="78" t="s">
         <v>42</v>
       </c>
+      <c r="J46" s="65"/>
     </row>
-    <row r="47" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="66"/>
-      <c r="D47" s="66"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="73"/>
-      <c r="H47" s="73"/>
-      <c r="I47" s="73"/>
+    <row r="47" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="63"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="98"/>
+      <c r="F47" s="78"/>
+      <c r="G47" s="78"/>
+      <c r="H47" s="78"/>
+      <c r="I47" s="78"/>
+      <c r="J47" s="65"/>
     </row>
-    <row r="48" spans="3:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="C48" s="66"/>
-      <c r="D48" s="66"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="73"/>
+    <row r="48" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="63"/>
+      <c r="C48" s="75"/>
+      <c r="D48" s="75"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="65"/>
     </row>
-    <row r="49" spans="3:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="66"/>
-      <c r="D49" s="66"/>
-      <c r="E49" s="29" t="s">
+    <row r="49" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="63"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F49" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="G49" s="22" t="s">
+      <c r="G49" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="H49" s="22" t="s">
+      <c r="H49" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="I49" s="22" t="s">
+      <c r="I49" s="21" t="s">
         <v>47</v>
       </c>
+      <c r="J49" s="65"/>
     </row>
-    <row r="50" spans="3:12" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="52" t="s">
+    <row r="50" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="63"/>
+      <c r="C50" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="41" t="s">
+      <c r="D50" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="E50" s="43" t="s">
+      <c r="E50" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="F50" s="58" t="s">
+      <c r="F50" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="G50" s="43" t="s">
+      <c r="G50" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H50" s="63" t="s">
+      <c r="H50" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="I50" s="44" t="s">
+      <c r="I50" s="41" t="s">
         <v>69</v>
       </c>
+      <c r="J50" s="65"/>
     </row>
-    <row r="51" spans="3:12" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="52"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="22"/>
+    <row r="51" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="63"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="65"/>
     </row>
-    <row r="52" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="65"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="65"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="65"/>
-      <c r="L52" s="46"/>
+    <row r="52" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="63"/>
+      <c r="D52" s="97"/>
+      <c r="E52" s="97"/>
+      <c r="F52" s="97"/>
+      <c r="G52" s="97"/>
+      <c r="H52" s="97"/>
+      <c r="J52" s="65"/>
+      <c r="L52" s="43"/>
     </row>
-    <row r="53" spans="3:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="26" t="s">
+    <row r="53" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="63"/>
+      <c r="D53" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="E53" s="47" t="s">
+      <c r="E53" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G53" s="22" t="s">
+      <c r="G53" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="H53" s="17" t="s">
+      <c r="H53" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I53" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="L53" s="46"/>
+      <c r="J53" s="65"/>
+      <c r="L53" s="43"/>
     </row>
-    <row r="54" spans="3:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G54" s="22" t="s">
+    <row r="54" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="63"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="99"/>
+      <c r="G54" s="81"/>
+      <c r="H54" s="102"/>
+      <c r="I54" s="104"/>
+      <c r="J54" s="65"/>
+      <c r="L54" s="43"/>
+    </row>
+    <row r="55" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="63"/>
+      <c r="G55" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="H54" s="17" t="s">
+      <c r="H55" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="I54" s="9" t="s">
+      <c r="I55" s="103" t="s">
         <v>50</v>
       </c>
+      <c r="J55" s="65"/>
     </row>
-    <row r="55" spans="3:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G55" s="23"/>
-      <c r="H55" s="48"/>
+    <row r="56" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="63"/>
+      <c r="G56" s="78"/>
+      <c r="H56" s="100"/>
+      <c r="I56" s="103"/>
+      <c r="J56" s="65"/>
     </row>
-    <row r="56" spans="3:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G56" s="23"/>
-      <c r="H56" s="48"/>
+    <row r="57" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="63"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="44"/>
+      <c r="J57" s="65"/>
     </row>
-    <row r="58" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E58" s="49"/>
-      <c r="G58" s="50"/>
+    <row r="58" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="63"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="44"/>
+      <c r="J58" s="65"/>
     </row>
-    <row r="59" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
+    <row r="59" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="68"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="69"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="69"/>
+      <c r="G59" s="69"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="69"/>
+      <c r="J59" s="65"/>
     </row>
-    <row r="60" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
+    <row r="60" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="72"/>
+      <c r="E60" s="45"/>
+      <c r="G60" s="46"/>
+      <c r="J60" s="65"/>
+      <c r="K60" s="71"/>
     </row>
-    <row r="61" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
+    <row r="61" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="71"/>
+      <c r="E61" s="45"/>
+      <c r="G61" s="46"/>
+      <c r="J61" s="65"/>
+      <c r="K61" s="71"/>
     </row>
-    <row r="62" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
+    <row r="62" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="71"/>
+      <c r="E62" s="45"/>
+      <c r="G62" s="46"/>
+      <c r="J62" s="65"/>
+      <c r="K62" s="71"/>
     </row>
-    <row r="63" spans="3:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
+    <row r="63" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="71"/>
+      <c r="E63" s="45"/>
+      <c r="G63" s="46"/>
+      <c r="J63" s="65"/>
+      <c r="K63" s="71"/>
+    </row>
+    <row r="64" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="71"/>
+      <c r="E64" s="45"/>
+      <c r="G64" s="46"/>
+      <c r="J64" s="65"/>
+      <c r="K64" s="71"/>
+    </row>
+    <row r="65" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="71"/>
+      <c r="E65" s="45"/>
+      <c r="G65" s="46"/>
+      <c r="J65" s="65"/>
+      <c r="K65" s="71"/>
+    </row>
+    <row r="66" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="71"/>
+      <c r="E66" s="45"/>
+      <c r="G66" s="46"/>
+      <c r="J66" s="65"/>
+      <c r="K66" s="71"/>
+    </row>
+    <row r="67" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="71"/>
+      <c r="E67" s="45"/>
+      <c r="G67" s="46"/>
+      <c r="J67" s="65"/>
+      <c r="K67" s="71"/>
+    </row>
+    <row r="68" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="71"/>
+      <c r="E68" s="45"/>
+      <c r="G68" s="46"/>
+      <c r="J68" s="65"/>
+      <c r="K68" s="71"/>
+    </row>
+    <row r="69" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="71"/>
+      <c r="E69" s="45"/>
+      <c r="G69" s="46"/>
+      <c r="J69" s="65"/>
+      <c r="K69" s="71"/>
+    </row>
+    <row r="70" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="71"/>
+      <c r="E70" s="45"/>
+      <c r="G70" s="46"/>
+      <c r="J70" s="65"/>
+      <c r="K70" s="71"/>
+    </row>
+    <row r="71" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="71"/>
+      <c r="E71" s="45"/>
+      <c r="G71" s="46"/>
+      <c r="J71" s="65"/>
+      <c r="K71" s="71"/>
+    </row>
+    <row r="72" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="71"/>
+      <c r="E72" s="45"/>
+      <c r="G72" s="46"/>
+      <c r="J72" s="65"/>
+      <c r="K72" s="71"/>
+    </row>
+    <row r="73" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="71"/>
+      <c r="E73" s="45"/>
+      <c r="G73" s="46"/>
+      <c r="J73" s="65"/>
+      <c r="K73" s="71"/>
+    </row>
+    <row r="74" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="71"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="70"/>
+    </row>
+    <row r="75" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="K75" s="71"/>
+    </row>
+    <row r="76" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="I28:I33"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B1:C3"/>
-    <mergeCell ref="E1:H3"/>
-    <mergeCell ref="C24:D25"/>
-    <mergeCell ref="E24:E25"/>
+  <mergeCells count="33">
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="I53:I54"/>
     <mergeCell ref="D52:H52"/>
     <mergeCell ref="C27:C34"/>
     <mergeCell ref="D27:D34"/>
@@ -30832,6 +31082,18 @@
     <mergeCell ref="F46:F48"/>
     <mergeCell ref="G46:G48"/>
     <mergeCell ref="H46:H48"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="I28:I33"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B1:C3"/>
+    <mergeCell ref="E1:H3"/>
+    <mergeCell ref="C24:D25"/>
+    <mergeCell ref="E24:E25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.15748031496062992" footer="0.15748031496062992"/>

</xml_diff>